<commit_message>
Test de modelo terminados: Se terminan los test de modelo
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -1728,7 +1728,7 @@
   <dimension ref="B6:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1827,7 @@
       <c r="E15" s="15">
         <v>5</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       <c r="E16" s="15">
         <v>6</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="17" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
       <c r="E17" s="15">
         <v>7</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       <c r="E18" s="15">
         <v>8</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="17" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modelo de Usuario y producto terminado
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -189,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +244,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -285,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -330,6 +336,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1728,7 +1735,7 @@
   <dimension ref="B6:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,7 +1785,7 @@
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="15">
@@ -1788,12 +1795,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="17"/>
+    </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="15">
@@ -1807,7 +1816,7 @@
       <c r="B14" s="15">
         <v>4</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="18" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="15">
@@ -1821,7 +1830,7 @@
       <c r="B15" s="15">
         <v>5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="15">

</xml_diff>

<commit_message>
Modelo de inventarios y atencion
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="2"/>
@@ -11,7 +11,7 @@
     <sheet name="cronograma" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1735,7 +1735,7 @@
   <dimension ref="B6:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,7 +1844,7 @@
       <c r="B16" s="15">
         <v>6</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="15">

</xml_diff>

<commit_message>
Modelo AtencionProducto y lista de view en el cronograma
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="2"/>
@@ -11,12 +11,12 @@
     <sheet name="cronograma" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>Actividad</t>
   </si>
@@ -145,13 +145,82 @@
   </si>
   <si>
     <t>Test Orden</t>
+  </si>
+  <si>
+    <t>Vistas  lista</t>
+  </si>
+  <si>
+    <t>Vistas Orden</t>
+  </si>
+  <si>
+    <t>Login sistema</t>
+  </si>
+  <si>
+    <t>login usuario</t>
+  </si>
+  <si>
+    <t>menu principal</t>
+  </si>
+  <si>
+    <t>Pedido selección mesa</t>
+  </si>
+  <si>
+    <t>Pedido Selección Productos</t>
+  </si>
+  <si>
+    <t>caja listado de pedidos</t>
+  </si>
+  <si>
+    <t>pago de pedido</t>
+  </si>
+  <si>
+    <t>cocina lista de pedidos</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>inicio administracion</t>
+  </si>
+  <si>
+    <t>admin crud usuarios</t>
+  </si>
+  <si>
+    <t>admin crud mesas</t>
+  </si>
+  <si>
+    <t>admin crud categorias</t>
+  </si>
+  <si>
+    <t>admin crud productos</t>
+  </si>
+  <si>
+    <t>admin atenciones</t>
+  </si>
+  <si>
+    <t>admin reportes</t>
+  </si>
+  <si>
+    <t>detalle del pedido</t>
+  </si>
+  <si>
+    <t>pedidos de determinado usuario</t>
+  </si>
+  <si>
+    <t>cuentas abiertas</t>
+  </si>
+  <si>
+    <t>mensajeria</t>
+  </si>
+  <si>
+    <t>perfil de usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +253,14 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -337,6 +414,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +719,7 @@
   <dimension ref="B5:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,16 +1810,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F18"/>
+  <dimension ref="B6:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="15"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="15" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" style="15"/>
     <col min="6" max="6" width="19" style="15" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="15"/>
@@ -1858,7 +1936,7 @@
       <c r="B17" s="15">
         <v>7</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="15">
@@ -1872,7 +1950,7 @@
       <c r="B18" s="15">
         <v>8</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="15">
@@ -1880,6 +1958,182 @@
       </c>
       <c r="F18" s="17" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
+        <v>1</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
+        <v>3</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="15">
+        <v>4</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="15">
+        <v>6</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="15">
+        <v>7</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="15">
+        <v>8</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="15">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="15">
+        <v>10</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="15">
+        <v>11</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="15">
+        <v>12</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>13</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="15">
+        <v>14</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
+        <v>15</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="15">
+        <v>16</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="15">
+        <v>17</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="15">
+        <v>18</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="15">
+        <v>19</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="15">
+        <v>20</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="15">
+        <v>21</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agrega nuevo cronograma,elimina modelos y test
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>Actividad</t>
   </si>
@@ -142,13 +142,85 @@
   </si>
   <si>
     <t>AtencionProducto</t>
+  </si>
+  <si>
+    <t>Test Orden</t>
+  </si>
+  <si>
+    <t>Vistas  lista</t>
+  </si>
+  <si>
+    <t>Vistas Orden</t>
+  </si>
+  <si>
+    <t>Login sistema</t>
+  </si>
+  <si>
+    <t>login usuario</t>
+  </si>
+  <si>
+    <t>menu principal</t>
+  </si>
+  <si>
+    <t>Pedido selección mesa</t>
+  </si>
+  <si>
+    <t>Pedido Selección Productos</t>
+  </si>
+  <si>
+    <t>caja listado de pedidos</t>
+  </si>
+  <si>
+    <t>pago de pedido</t>
+  </si>
+  <si>
+    <t>cocina lista de pedidos</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>inicio administracion</t>
+  </si>
+  <si>
+    <t>admin crud usuarios</t>
+  </si>
+  <si>
+    <t>admin crud mesas</t>
+  </si>
+  <si>
+    <t>admin crud categorias</t>
+  </si>
+  <si>
+    <t>admin crud productos</t>
+  </si>
+  <si>
+    <t>admin atenciones</t>
+  </si>
+  <si>
+    <t>admin reportes</t>
+  </si>
+  <si>
+    <t>detalle del pedido</t>
+  </si>
+  <si>
+    <t>pedidos de determinado usuario</t>
+  </si>
+  <si>
+    <t>cuentas abiertas</t>
+  </si>
+  <si>
+    <t>mensajeria</t>
+  </si>
+  <si>
+    <t>perfil de usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,8 +257,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +315,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -276,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -320,6 +412,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +719,7 @@
   <dimension ref="B5:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,94 +1810,330 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:C18"/>
+  <dimension ref="B6:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="15"/>
-    <col min="3" max="3" width="19" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="15"/>
+    <col min="3" max="3" width="25.7109375" style="15" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="15"/>
+    <col min="6" max="6" width="19" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F6" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="F8" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="15">
+        <v>2</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="15">
+        <v>3</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <v>4</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="15">
+        <v>4</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="15">
         <v>5</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="15">
+        <v>5</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>6</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="15">
+        <v>6</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>7</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="15">
+        <v>7</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <v>8</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="17" t="s">
         <v>41</v>
+      </c>
+      <c r="E18" s="15">
+        <v>8</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="15">
+        <v>1</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="15">
+        <v>2</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="15">
+        <v>3</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="15">
+        <v>4</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="15">
+        <v>5</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="15">
+        <v>6</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="15">
+        <v>7</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="15">
+        <v>8</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="15">
+        <v>9</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="15">
+        <v>10</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="15">
+        <v>11</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="15">
+        <v>12</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="15">
+        <v>13</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="15">
+        <v>14</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="15">
+        <v>15</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="15">
+        <v>16</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="15">
+        <v>17</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="15">
+        <v>18</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="15">
+        <v>19</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="15">
+        <v>20</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="15">
+        <v>21</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregaron librerias de la plantilla , se creo la pagina principal vacia
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Actividad</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Test Orden</t>
   </si>
   <si>
-    <t>Vistas  lista</t>
-  </si>
-  <si>
     <t>Vistas Orden</t>
   </si>
   <si>
@@ -168,15 +165,9 @@
     <t>Pedido Selección Productos</t>
   </si>
   <si>
-    <t>caja listado de pedidos</t>
-  </si>
-  <si>
     <t>pago de pedido</t>
   </si>
   <si>
-    <t>cocina lista de pedidos</t>
-  </si>
-  <si>
     <t>inventario</t>
   </si>
   <si>
@@ -214,6 +205,21 @@
   </si>
   <si>
     <t>perfil de usuario</t>
+  </si>
+  <si>
+    <t>blank page</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>caja</t>
+  </si>
+  <si>
+    <t>cocina</t>
   </si>
 </sst>
 </file>
@@ -1810,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F45"/>
+  <dimension ref="B6:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,153 +1966,158 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>44</v>
+      <c r="B24" s="15">
+        <v>1</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="15">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="15">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="15">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="15">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>57</v>
@@ -2114,26 +2125,42 @@
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="15">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="15">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="15">
+        <v>23</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="15">
+        <v>24</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vista Pedidos_producto terminada, tambien pedido_mesas y login
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -272,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +333,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -421,6 +427,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1818,15 +1825,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="15"/>
     <col min="3" max="3" width="25.7109375" style="15" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="15"/>
+    <col min="4" max="4" width="3.5703125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="15"/>
     <col min="6" max="6" width="19" style="15" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" style="15"/>
   </cols>
@@ -1975,7 +1983,7 @@
       <c r="B24" s="15">
         <v>1</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1983,7 +1991,7 @@
       <c r="B25" s="15">
         <v>2</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="17" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1991,7 +1999,7 @@
       <c r="B26" s="15">
         <v>3</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="17" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1999,7 +2007,7 @@
       <c r="B27" s="15">
         <v>4</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2007,7 +2015,7 @@
       <c r="B28" s="15">
         <v>5</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2015,7 +2023,7 @@
       <c r="B29" s="15">
         <v>6</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2023,9 +2031,10 @@
       <c r="B30" s="15">
         <v>7</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="17" t="s">
         <v>48</v>
       </c>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="15">
@@ -2034,6 +2043,7 @@
       <c r="C31" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="D31" s="20"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="15">
@@ -2043,7 +2053,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="15">
         <v>10</v>
       </c>
@@ -2051,15 +2061,16 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="15">
         <v>11</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="20"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="15">
         <v>12</v>
       </c>
@@ -2067,15 +2078,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="15">
         <v>13</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="15">
         <v>14</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="15">
         <v>15</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="15">
         <v>16</v>
       </c>
@@ -2099,7 +2111,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="15">
         <v>17</v>
       </c>
@@ -2107,23 +2119,25 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="15">
         <v>18</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="15">
         <v>19</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="15">
         <v>20</v>
       </c>
@@ -2131,7 +2145,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="15">
         <v>21</v>
       </c>
@@ -2139,7 +2153,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="15">
         <v>22</v>
       </c>
@@ -2147,7 +2161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="15">
         <v>23</v>
       </c>
@@ -2155,7 +2169,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="15">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Vistas caja y cocina
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -380,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -428,6 +428,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1826,7 +1827,7 @@
   <dimension ref="B6:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2041,7 @@
       <c r="B31" s="15">
         <v>8</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="21" t="s">
         <v>45</v>
       </c>
       <c r="D31" s="20"/>
@@ -2049,7 +2050,7 @@
       <c r="B32" s="15">
         <v>9</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="17" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2057,7 +2058,7 @@
       <c r="B33" s="15">
         <v>10</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="17" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vistas de inventarios,cuentas abiertas ,pedidos usuario y perfil
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="2"/>
@@ -11,12 +11,12 @@
     <sheet name="cronograma" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Actividad</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>cocina</t>
+  </si>
+  <si>
+    <t>Mensajeria</t>
   </si>
 </sst>
 </file>
@@ -838,7 +841,7 @@
   <dimension ref="A1:BA207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,16 +1827,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F47"/>
+  <dimension ref="B6:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="15"/>
-    <col min="3" max="3" width="25.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" style="15" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="15"/>
     <col min="6" max="6" width="19" style="15" customWidth="1"/>
@@ -1947,7 +1950,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>7</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <v>8</v>
       </c>
@@ -1975,12 +1978,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C23" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="15">
         <v>1</v>
       </c>
@@ -1988,15 +1991,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15">
         <v>2</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H25" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="15">
         <v>3</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="15">
         <v>4</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="15">
         <v>5</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="15">
         <v>6</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="15">
         <v>7</v>
       </c>
@@ -2037,7 +2043,7 @@
       </c>
       <c r="D30" s="20"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="15">
         <v>8</v>
       </c>
@@ -2046,7 +2052,7 @@
       </c>
       <c r="D31" s="20"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="15">
         <v>9</v>
       </c>
@@ -2075,7 +2081,7 @@
       <c r="B35" s="15">
         <v>12</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="17" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2083,7 +2089,7 @@
       <c r="B36" s="15">
         <v>13</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="17" t="s">
         <v>50</v>
       </c>
       <c r="D36" s="20"/>
@@ -2092,7 +2098,7 @@
       <c r="B37" s="15">
         <v>14</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="17" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2100,7 +2106,7 @@
       <c r="B38" s="15">
         <v>15</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="17" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2108,7 +2114,7 @@
       <c r="B39" s="15">
         <v>16</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="17" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Vista admin inicio,admin reportes dia y fecha
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -1830,7 +1830,7 @@
   <dimension ref="B6:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41:C42"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2130,7 +2130,7 @@
       <c r="B41" s="15">
         <v>18</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D41" s="20"/>
@@ -2139,7 +2139,7 @@
       <c r="B42" s="15">
         <v>19</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D42" s="20"/>
@@ -2157,7 +2157,7 @@
         <v>21</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
         <v>22</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -2173,7 +2173,7 @@
         <v>23</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
         <v>24</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base de datos, cambio de nombres a tablas y a modelos , se hacen pruebas
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="18915" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actidades" sheetId="1" r:id="rId1"/>
     <sheet name="cronograma" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="orden" sheetId="3" r:id="rId3"/>
+    <sheet name="entradas y salidas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="121">
   <si>
     <t>Actividad</t>
   </si>
@@ -147,9 +148,6 @@
     <t>Test Orden</t>
   </si>
   <si>
-    <t>Vistas  lista</t>
-  </si>
-  <si>
     <t>Vistas Orden</t>
   </si>
   <si>
@@ -168,15 +166,9 @@
     <t>Pedido Selección Productos</t>
   </si>
   <si>
-    <t>caja listado de pedidos</t>
-  </si>
-  <si>
     <t>pago de pedido</t>
   </si>
   <si>
-    <t>cocina lista de pedidos</t>
-  </si>
-  <si>
     <t>inventario</t>
   </si>
   <si>
@@ -210,17 +202,191 @@
     <t>cuentas abiertas</t>
   </si>
   <si>
-    <t>mensajeria</t>
-  </si>
-  <si>
     <t>perfil de usuario</t>
+  </si>
+  <si>
+    <t>blank page</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>caja</t>
+  </si>
+  <si>
+    <t>cocina</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>controladores</t>
+  </si>
+  <si>
+    <t>Vista</t>
+  </si>
+  <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>Procesos</t>
+  </si>
+  <si>
+    <t>Salidas</t>
+  </si>
+  <si>
+    <t>pedidos del usuario</t>
+  </si>
+  <si>
+    <t>Validar usuario que ingresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json: usuario ,clave </t>
+  </si>
+  <si>
+    <t>controlador</t>
+  </si>
+  <si>
+    <t>lista de perfiles</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>mesa</t>
+  </si>
+  <si>
+    <t>Mesa,Categorias,Productos,Atenciones</t>
+  </si>
+  <si>
+    <t>Mesas,Estado</t>
+  </si>
+  <si>
+    <t>seleccionar pedido</t>
+  </si>
+  <si>
+    <t>json: pedido</t>
+  </si>
+  <si>
+    <t>mesa selecconada</t>
+  </si>
+  <si>
+    <t>perfil seleccionado</t>
+  </si>
+  <si>
+    <t>lista de pedidos de las ultimas horas</t>
+  </si>
+  <si>
+    <t>pedido seleccinado</t>
+  </si>
+  <si>
+    <t>atencion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lista de pedidos no despachados </t>
+  </si>
+  <si>
+    <t>pedido</t>
+  </si>
+  <si>
+    <t>facturar pedido</t>
+  </si>
+  <si>
+    <t>editar pedido</t>
+  </si>
+  <si>
+    <t>nuevo inventario</t>
+  </si>
+  <si>
+    <t>crear inventario</t>
+  </si>
+  <si>
+    <t>datos usuario,notificaciones</t>
+  </si>
+  <si>
+    <t>modificar inventario,crear notific</t>
+  </si>
+  <si>
+    <t>usuario,notificacion</t>
+  </si>
+  <si>
+    <t>Controlador pedido</t>
+  </si>
+  <si>
+    <t>pedidos categorias etc</t>
+  </si>
+  <si>
+    <t>pedidos</t>
+  </si>
+  <si>
+    <t>buscar reporte fecha</t>
+  </si>
+  <si>
+    <t>datos de usuario</t>
+  </si>
+  <si>
+    <t>crud usuario</t>
+  </si>
+  <si>
+    <t>datos usuario</t>
+  </si>
+  <si>
+    <t>datos de productos</t>
+  </si>
+  <si>
+    <t>crud productos</t>
+  </si>
+  <si>
+    <t>datos productos</t>
+  </si>
+  <si>
+    <t>datos atenciones</t>
+  </si>
+  <si>
+    <t>datos categorias</t>
+  </si>
+  <si>
+    <t>crud categorias</t>
+  </si>
+  <si>
+    <t>datos mesas</t>
+  </si>
+  <si>
+    <t>crud mesas</t>
+  </si>
+  <si>
+    <t>controlador estadisticas</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>atencione</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>controlador pedido</t>
+  </si>
+  <si>
+    <t>controlador estad</t>
+  </si>
+  <si>
+    <t>item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,8 +431,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +501,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -364,11 +544,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -415,6 +700,58 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,7 +1161,7 @@
   <dimension ref="A1:BA207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,42 +2147,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F45"/>
+  <dimension ref="B6:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="15"/>
-    <col min="3" max="3" width="25.7109375" style="15" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="15"/>
+    <col min="1" max="1" width="5" style="15" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="15"/>
     <col min="6" max="6" width="19" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="15"/>
+    <col min="7" max="7" width="12.140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="32" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="15"/>
+    <col min="11" max="11" width="2.85546875" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C6" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="15">
         <v>1</v>
       </c>
@@ -1858,8 +2214,15 @@
       <c r="F10" s="17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="15">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="38"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="15">
         <v>2</v>
       </c>
@@ -1872,11 +2235,35 @@
       <c r="F11" s="17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="15">
+        <v>2</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K11" s="15">
+        <v>1</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="15">
+        <v>3</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" s="15">
+        <v>2</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>3</v>
       </c>
@@ -1889,8 +2276,20 @@
       <c r="F13" s="17" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="15">
+        <v>4</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="15">
+        <v>3</v>
+      </c>
+      <c r="L13" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <v>4</v>
       </c>
@@ -1903,8 +2302,20 @@
       <c r="F14" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="15">
+        <v>5</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="15">
+        <v>4</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="15">
         <v>5</v>
       </c>
@@ -1917,8 +2328,20 @@
       <c r="F15" s="17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="15">
+        <v>6</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="15">
+        <v>5</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>6</v>
       </c>
@@ -1931,8 +2354,21 @@
       <c r="F16" s="17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="15">
+        <v>7</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="K16" s="15">
+        <v>6</v>
+      </c>
+      <c r="L16" s="38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>7</v>
       </c>
@@ -1945,8 +2381,21 @@
       <c r="F17" s="17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="15">
+        <v>8</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="K17" s="15">
+        <v>7</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="15">
         <v>8</v>
       </c>
@@ -1959,181 +2408,527 @@
       <c r="F18" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="G18" s="15">
+        <v>9</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="15">
+        <v>8</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G19" s="15">
+        <v>10</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="15">
+        <v>9</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="15">
+        <v>11</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="20"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G21" s="15">
+        <v>12</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="15">
+        <v>13</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="20"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G23" s="15">
+        <v>14</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G24" s="15">
+        <v>15</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G25" s="15">
+        <v>16</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="15">
+        <v>17</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G27" s="15">
+        <v>18</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G28" s="15">
+        <v>19</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="20"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G29" s="15">
+        <v>20</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G30" s="15">
+        <v>21</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G31" s="15">
+        <v>22</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="15">
+        <v>23</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="15">
+        <v>24</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="29" style="23" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" s="24" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="31"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>44</v>
+      <c r="D24" s="39" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15">
-        <v>1</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>45</v>
+      <c r="D25" s="23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="15">
-        <v>2</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>46</v>
+      <c r="D26" s="23" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="15">
-        <v>3</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>47</v>
+      <c r="B27" s="22"/>
+      <c r="D27" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="15">
-        <v>4</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>48</v>
+      <c r="B28" s="22"/>
+      <c r="D28" s="23" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="15">
-        <v>5</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>49</v>
+      <c r="B29" s="22"/>
+      <c r="D29" s="23" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="15">
-        <v>6</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>50</v>
+      <c r="B30" s="22"/>
+      <c r="D30" s="23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="15">
-        <v>7</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="15">
-        <v>8</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="15">
-        <v>9</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="15">
-        <v>10</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="15">
-        <v>11</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
-        <v>12</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="15">
-        <v>13</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="15">
-        <v>14</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="15">
-        <v>15</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="15">
-        <v>16</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="15">
-        <v>17</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="15">
-        <v>18</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="15">
-        <v>19</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="15">
-        <v>20</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="15">
-        <v>21</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>60</v>
+      <c r="B31" s="22"/>
+      <c r="D31" s="23" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
controladores de categoria e inicio de usuarios,faltan crud usuarios
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="121">
   <si>
     <t>Actividad</t>
   </si>
@@ -226,9 +226,6 @@
     <t>controladores</t>
   </si>
   <si>
-    <t>Vista</t>
-  </si>
-  <si>
     <t>Entradas</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>usuario,notificacion</t>
   </si>
   <si>
-    <t>Controlador pedido</t>
-  </si>
-  <si>
     <t>pedidos categorias etc</t>
   </si>
   <si>
@@ -364,9 +358,6 @@
     <t>producto</t>
   </si>
   <si>
-    <t>atencione</t>
-  </si>
-  <si>
     <t>categoria</t>
   </si>
   <si>
@@ -380,6 +371,15 @@
   </si>
   <si>
     <t>item</t>
+  </si>
+  <si>
+    <t>Vista / proceso</t>
+  </si>
+  <si>
+    <t>Sesiones</t>
+  </si>
+  <si>
+    <t>crear y eliminar Sesiones</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +510,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -768,6 +780,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2436,7 +2488,7 @@
         <v>8</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -2450,7 +2502,7 @@
         <v>9</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
@@ -2577,10 +2629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F31"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B18" sqref="B18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,354 +2650,367 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" s="24" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="E2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>72</v>
-      </c>
       <c r="F2" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="48" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="55" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="28" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="38" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="28"/>
+        <v>79</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>81</v>
+      </c>
       <c r="E7" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="28" t="s">
         <v>87</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="26"/>
+        <v>88</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="F9" s="28" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C10" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="E10" s="26"/>
       <c r="F10" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>93</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E11" s="26"/>
       <c r="F11" s="28" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="26"/>
+        <v>50</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>92</v>
+      </c>
       <c r="F12" s="28" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="26"/>
       <c r="F13" s="28" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="26" t="s">
-        <v>97</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="28" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="33" t="s">
-        <v>113</v>
+        <v>94</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>101</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D16" s="28"/>
       <c r="E16" s="26"/>
-      <c r="F16" s="28" t="s">
-        <v>88</v>
+      <c r="F16" s="33" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C18" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>114</v>
+      <c r="F18" s="56" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="26"/>
+        <v>103</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>105</v>
+      </c>
       <c r="F19" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C21" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D22" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E22" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="35" t="s">
-        <v>117</v>
+      <c r="F22" s="42" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D26" s="49" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="23" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="49" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
-      <c r="D27" s="23" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="22"/>
       <c r="D28" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="22"/>
       <c r="D29" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="22"/>
       <c r="D30" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="22"/>
       <c r="D31" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+      <c r="D32" s="23" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Controlador de usuario terminado y actualizacion de controlador de mesa y categoria
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -2632,7 +2632,7 @@
   <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:F18"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,19 +2844,19 @@
       </c>
     </row>
     <row r="15" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="56" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3011,7 +3011,7 @@
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="22"/>
       <c r="D32" s="23" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
controlador atencion , terminado pedido_productos
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -440,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +534,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -859,6 +865,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2671,7 +2689,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,25 +2787,25 @@
       <c r="B7" s="23">
         <v>1</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="69" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>65</v>
@@ -2838,7 +2856,7 @@
     </row>
     <row r="11" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>58</v>
@@ -2873,7 +2891,7 @@
     </row>
     <row r="13" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="25" t="s">
         <v>72</v>
@@ -2888,6 +2906,9 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23">
+        <v>7</v>
+      </c>
       <c r="C14" s="25" t="s">
         <v>60</v>
       </c>
@@ -2897,7 +2918,7 @@
       <c r="E14" s="28"/>
       <c r="F14" s="26"/>
       <c r="G14" s="28" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -2931,9 +2952,6 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="23">
-        <v>7</v>
-      </c>
       <c r="C17" s="25" t="s">
         <v>57</v>
       </c>
@@ -2984,7 +3002,7 @@
     </row>
     <row r="20" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
controlador atencion detallePedido update
</commit_message>
<xml_diff>
--- a/Modeler/CronogramaGeneral.xlsx
+++ b/Modeler/CronogramaGeneral.xlsx
@@ -2689,7 +2689,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,17 +2807,17 @@
       <c r="B8" s="23">
         <v>4</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="26" t="s">
+      <c r="E8" s="69"/>
+      <c r="F8" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="69" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2840,17 +2840,17 @@
       <c r="B10" s="23">
         <v>2</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="70"/>
+      <c r="G10" s="69" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>